<commit_message>
Sync file from Google Drive
</commit_message>
<xml_diff>
--- a/path/in/repo/DDP_OUTPUT.xlsx
+++ b/path/in/repo/DDP_OUTPUT.xlsx
@@ -461,114 +461,114 @@
   </sheetPr>
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>NextBusGroup</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>BusNo</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>BusStopCode</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Destination Description</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Operator</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>EstimatedTimeOfArrival</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>DestinationCode</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>WheelchairAccessible</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>Load</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>Monitored</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>OriginCode</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>TypeOfBus</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>Right_BusStopCode</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>SAT_FirstBus</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" s="3" t="inlineStr">
         <is>
           <t>SAT_LastBus</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" s="3" t="inlineStr">
         <is>
           <t>SUN_FirstBus</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" s="3" t="inlineStr">
         <is>
           <t>SUN_LastBus</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" s="3" t="inlineStr">
         <is>
           <t>WD_FirstBus</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" s="3" t="inlineStr">
         <is>
           <t>WD_LastBus</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" s="3" t="inlineStr">
         <is>
           <t>Right_Right_BusStopCode</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" s="3" t="inlineStr">
         <is>
           <t>Bus Stop Description</t>
         </is>
@@ -580,15 +580,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>53009</t>
-        </is>
+      <c r="B2" t="n">
+        <v>52</v>
+      </c>
+      <c r="C2" t="n">
+        <v>53009</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -600,13 +596,11 @@
           <t>SBST</t>
         </is>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>45683.9718287037</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>53009</t>
-        </is>
+      <c r="F2" s="5" t="n">
+        <v>45684.38576388889</v>
+      </c>
+      <c r="G2" t="n">
+        <v>53009</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -618,60 +612,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>28009</t>
-        </is>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>28009</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>SD</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>0612</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>0015</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>0613</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>0016</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>0619</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>0015</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
+          <t>DD</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>12101</v>
+      </c>
+      <c r="N2" t="n">
+        <v>612</v>
+      </c>
+      <c r="O2" t="n">
+        <v>15</v>
+      </c>
+      <c r="P2" t="n">
+        <v>613</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>16</v>
+      </c>
+      <c r="R2" t="n">
+        <v>619</v>
+      </c>
+      <c r="S2" t="n">
+        <v>15</v>
+      </c>
+      <c r="T2" t="n">
+        <v>12101</v>
       </c>
       <c r="U2" t="inlineStr">
         <is>
@@ -685,15 +659,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>184</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>44989</t>
-        </is>
+      <c r="B3" t="n">
+        <v>184</v>
+      </c>
+      <c r="C3" t="n">
+        <v>44989</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -705,13 +675,11 @@
           <t>SMRT</t>
         </is>
       </c>
-      <c r="F3" s="2" t="n">
-        <v>45683.96837962963</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>44989</t>
-        </is>
+      <c r="F3" s="5" t="n">
+        <v>45684.38296296296</v>
+      </c>
+      <c r="G3" t="n">
+        <v>44989</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -723,60 +691,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>44989</t>
-        </is>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>44989</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>SD</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>0622</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>2331</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>0621</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>2331</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>0602</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>2327</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
+          <t>DD</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>12109</v>
+      </c>
+      <c r="N3" t="n">
+        <v>622</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2331</v>
+      </c>
+      <c r="P3" t="n">
+        <v>621</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2331</v>
+      </c>
+      <c r="R3" t="n">
+        <v>602</v>
+      </c>
+      <c r="S3" t="n">
+        <v>2327</v>
+      </c>
+      <c r="T3" t="n">
+        <v>12109</v>
       </c>
       <c r="U3" t="inlineStr">
         <is>
@@ -790,15 +738,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>44989</t>
-        </is>
+      <c r="B4" t="n">
+        <v>75</v>
+      </c>
+      <c r="C4" t="n">
+        <v>44989</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -810,13 +754,11 @@
           <t>SMRT</t>
         </is>
       </c>
-      <c r="F4" s="2" t="n">
-        <v>45683.97491898148</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>44989</t>
-        </is>
+      <c r="F4" s="5" t="n">
+        <v>45684.3840625</v>
+      </c>
+      <c r="G4" t="n">
+        <v>44989</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -828,60 +770,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>10009</t>
-        </is>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>10009</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>SD</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>0640</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>0032</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>0704</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>0030</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>0633</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>0031</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
+      <c r="M4" t="n">
+        <v>12101</v>
+      </c>
+      <c r="N4" t="n">
+        <v>640</v>
+      </c>
+      <c r="O4" t="n">
+        <v>32</v>
+      </c>
+      <c r="P4" t="n">
+        <v>704</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>30</v>
+      </c>
+      <c r="R4" t="n">
+        <v>633</v>
+      </c>
+      <c r="S4" t="n">
+        <v>31</v>
+      </c>
+      <c r="T4" t="n">
+        <v>12101</v>
       </c>
       <c r="U4" t="inlineStr">
         <is>
@@ -895,15 +817,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>184</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>44989</t>
-        </is>
+      <c r="B5" t="n">
+        <v>184</v>
+      </c>
+      <c r="C5" t="n">
+        <v>44989</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -915,13 +833,11 @@
           <t>SMRT</t>
         </is>
       </c>
-      <c r="F5" s="2" t="n">
-        <v>45683.96752314815</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>44989</t>
-        </is>
+      <c r="F5" s="5" t="n">
+        <v>45684.390625</v>
+      </c>
+      <c r="G5" t="n">
+        <v>44989</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -933,60 +849,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>44989</t>
-        </is>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>44989</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>SD</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>0638</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>2347</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>0634</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>2345</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>0612</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>2350</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
+          <t>DD</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>12101</v>
+      </c>
+      <c r="N5" t="n">
+        <v>638</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2347</v>
+      </c>
+      <c r="P5" t="n">
+        <v>634</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>2345</v>
+      </c>
+      <c r="R5" t="n">
+        <v>612</v>
+      </c>
+      <c r="S5" t="n">
+        <v>2350</v>
+      </c>
+      <c r="T5" t="n">
+        <v>12101</v>
       </c>
       <c r="U5" t="inlineStr">
         <is>
@@ -1000,15 +896,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>74</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>11379</t>
-        </is>
+      <c r="B6" t="n">
+        <v>74</v>
+      </c>
+      <c r="C6" t="n">
+        <v>11379</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1020,13 +912,11 @@
           <t>SBST</t>
         </is>
       </c>
-      <c r="F6" s="2" t="n">
-        <v>45683.97078703704</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>11379</t>
-        </is>
+      <c r="F6" s="5" t="n">
+        <v>45684.38430555556</v>
+      </c>
+      <c r="G6" t="n">
+        <v>11379</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -1038,60 +928,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>64009</t>
-        </is>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>64009</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>DD</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>0605</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>0030</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>0559</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>0024</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>0609</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>0027</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
+      <c r="M6" t="n">
+        <v>12109</v>
+      </c>
+      <c r="N6" t="n">
+        <v>605</v>
+      </c>
+      <c r="O6" t="n">
+        <v>30</v>
+      </c>
+      <c r="P6" t="n">
+        <v>559</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>24</v>
+      </c>
+      <c r="R6" t="n">
+        <v>609</v>
+      </c>
+      <c r="S6" t="n">
+        <v>27</v>
+      </c>
+      <c r="T6" t="n">
+        <v>12109</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
@@ -1105,15 +975,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>82009</t>
-        </is>
+      <c r="B7" t="n">
+        <v>61</v>
+      </c>
+      <c r="C7" t="n">
+        <v>82009</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1125,13 +991,11 @@
           <t>SMRT</t>
         </is>
       </c>
-      <c r="F7" s="2" t="n">
-        <v>45683.971875</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>82009</t>
-        </is>
+      <c r="F7" s="5" t="n">
+        <v>45684.38376157408</v>
+      </c>
+      <c r="G7" t="n">
+        <v>82009</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -1143,60 +1007,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>43009</t>
-        </is>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>43009</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>SD</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>0538</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>2349</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>0538</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>2349</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>0538</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>2349</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
+      <c r="M7" t="n">
+        <v>12109</v>
+      </c>
+      <c r="N7" t="n">
+        <v>538</v>
+      </c>
+      <c r="O7" t="n">
+        <v>2349</v>
+      </c>
+      <c r="P7" t="n">
+        <v>538</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>2349</v>
+      </c>
+      <c r="R7" t="n">
+        <v>538</v>
+      </c>
+      <c r="S7" t="n">
+        <v>2349</v>
+      </c>
+      <c r="T7" t="n">
+        <v>12109</v>
       </c>
       <c r="U7" t="inlineStr">
         <is>
@@ -1210,15 +1054,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>154</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>82009</t>
-        </is>
+      <c r="B8" t="n">
+        <v>154</v>
+      </c>
+      <c r="C8" t="n">
+        <v>82009</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1230,13 +1070,11 @@
           <t>SBST</t>
         </is>
       </c>
-      <c r="F8" s="2" t="n">
-        <v>45683.96949074074</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>82009</t>
-        </is>
+      <c r="F8" s="5" t="n">
+        <v>45684.38396990741</v>
+      </c>
+      <c r="G8" t="n">
+        <v>82009</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1248,60 +1086,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>22009</t>
-        </is>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>22009</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>SD</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>0601</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>0057</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>0637</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>0055</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>0604</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>0053</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
+      <c r="M8" t="n">
+        <v>12101</v>
+      </c>
+      <c r="N8" t="n">
+        <v>601</v>
+      </c>
+      <c r="O8" t="n">
+        <v>57</v>
+      </c>
+      <c r="P8" t="n">
+        <v>637</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>55</v>
+      </c>
+      <c r="R8" t="n">
+        <v>604</v>
+      </c>
+      <c r="S8" t="n">
+        <v>53</v>
+      </c>
+      <c r="T8" t="n">
+        <v>12101</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
@@ -1315,15 +1133,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>154</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>22009</t>
-        </is>
+      <c r="B9" t="n">
+        <v>154</v>
+      </c>
+      <c r="C9" t="n">
+        <v>22009</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1335,13 +1149,11 @@
           <t>SBST</t>
         </is>
       </c>
-      <c r="F9" s="2" t="n">
-        <v>45683.97039351852</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>22009</t>
-        </is>
+      <c r="F9" s="5" t="n">
+        <v>45684.38815972222</v>
+      </c>
+      <c r="G9" t="n">
+        <v>22009</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1353,60 +1165,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>82009</t>
-        </is>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>82009</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>DD</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>0546</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>0016</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>0616</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>0015</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>0547</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>0015</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>12109</v>
+      </c>
+      <c r="N9" t="n">
+        <v>546</v>
+      </c>
+      <c r="O9" t="n">
+        <v>16</v>
+      </c>
+      <c r="P9" t="n">
+        <v>616</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>15</v>
+      </c>
+      <c r="R9" t="n">
+        <v>547</v>
+      </c>
+      <c r="S9" t="n">
+        <v>15</v>
+      </c>
+      <c r="T9" t="n">
+        <v>12109</v>
       </c>
       <c r="U9" t="inlineStr">
         <is>
@@ -1420,15 +1212,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>43009</t>
-        </is>
+      <c r="B10" t="n">
+        <v>61</v>
+      </c>
+      <c r="C10" t="n">
+        <v>43009</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1440,13 +1228,11 @@
           <t>SMRT</t>
         </is>
       </c>
-      <c r="F10" s="2" t="n">
-        <v>45683.96637731481</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>43009</t>
-        </is>
+      <c r="F10" s="5" t="n">
+        <v>45684.38703703704</v>
+      </c>
+      <c r="G10" t="n">
+        <v>43009</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1458,60 +1244,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>82009</t>
-        </is>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
+        <v>82009</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
           <t>SD</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>0645</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>0108</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>0652</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>0110</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>0642</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>0109</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
+      <c r="M10" t="n">
+        <v>12101</v>
+      </c>
+      <c r="N10" t="n">
+        <v>645</v>
+      </c>
+      <c r="O10" t="n">
+        <v>108</v>
+      </c>
+      <c r="P10" t="n">
+        <v>652</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>110</v>
+      </c>
+      <c r="R10" t="n">
+        <v>642</v>
+      </c>
+      <c r="S10" t="n">
+        <v>109</v>
+      </c>
+      <c r="T10" t="n">
+        <v>12101</v>
       </c>
       <c r="U10" t="inlineStr">
         <is>
@@ -1525,15 +1291,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>74</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>64009</t>
-        </is>
+      <c r="B11" t="n">
+        <v>74</v>
+      </c>
+      <c r="C11" t="n">
+        <v>64009</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1545,13 +1307,11 @@
           <t>SBST</t>
         </is>
       </c>
-      <c r="F11" s="2" t="n">
-        <v>45683.96896990741</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>64009</t>
-        </is>
+      <c r="F11" s="5" t="n">
+        <v>45684.38572916666</v>
+      </c>
+      <c r="G11" t="n">
+        <v>64009</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1563,60 +1323,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>11379</t>
-        </is>
+      <c r="J11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" t="n">
+        <v>11379</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>SD</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>0602</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>2343</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>0623</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>2340</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>0549</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>2343</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
+          <t>DD</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>12101</v>
+      </c>
+      <c r="N11" t="n">
+        <v>602</v>
+      </c>
+      <c r="O11" t="n">
+        <v>2343</v>
+      </c>
+      <c r="P11" t="n">
+        <v>623</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2340</v>
+      </c>
+      <c r="R11" t="n">
+        <v>549</v>
+      </c>
+      <c r="S11" t="n">
+        <v>2343</v>
+      </c>
+      <c r="T11" t="n">
+        <v>12101</v>
       </c>
       <c r="U11" t="inlineStr">
         <is>
@@ -1630,15 +1370,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>64009</t>
-        </is>
+      <c r="B12" t="n">
+        <v>151</v>
+      </c>
+      <c r="C12" t="n">
+        <v>64009</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1650,13 +1386,11 @@
           <t>SBST</t>
         </is>
       </c>
-      <c r="F12" s="2" t="n">
-        <v>45683.96962962963</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>64009</t>
-        </is>
+      <c r="F12" s="5" t="n">
+        <v>45684.38391203704</v>
+      </c>
+      <c r="G12" t="n">
+        <v>64009</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1668,60 +1402,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>16009</t>
-        </is>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" t="n">
+        <v>16009</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
           <t>SD</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>0642</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>2317</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>0642</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>2315</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>0611</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>2317</t>
-        </is>
-      </c>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>12101</t>
-        </is>
+      <c r="M12" t="n">
+        <v>12101</v>
+      </c>
+      <c r="N12" t="n">
+        <v>642</v>
+      </c>
+      <c r="O12" t="n">
+        <v>2317</v>
+      </c>
+      <c r="P12" t="n">
+        <v>642</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>2315</v>
+      </c>
+      <c r="R12" t="n">
+        <v>611</v>
+      </c>
+      <c r="S12" t="n">
+        <v>2317</v>
+      </c>
+      <c r="T12" t="n">
+        <v>12101</v>
       </c>
       <c r="U12" t="inlineStr">
         <is>
@@ -1735,15 +1449,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>28009</t>
-        </is>
+      <c r="B13" t="n">
+        <v>52</v>
+      </c>
+      <c r="C13" t="n">
+        <v>28009</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1755,13 +1465,11 @@
           <t>SBST</t>
         </is>
       </c>
-      <c r="F13" s="2" t="n">
-        <v>45683.96574074074</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>28009</t>
-        </is>
+      <c r="F13" s="5" t="n">
+        <v>45684.38292824074</v>
+      </c>
+      <c r="G13" t="n">
+        <v>28009</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1773,60 +1481,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>53009</t>
-        </is>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>53009</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
           <t>SD</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>0623</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>0023</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>0625</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>0021</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>0627</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>0022</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
+      <c r="M13" t="n">
+        <v>12109</v>
+      </c>
+      <c r="N13" t="n">
+        <v>623</v>
+      </c>
+      <c r="O13" t="n">
+        <v>23</v>
+      </c>
+      <c r="P13" t="n">
+        <v>625</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>21</v>
+      </c>
+      <c r="R13" t="n">
+        <v>627</v>
+      </c>
+      <c r="S13" t="n">
+        <v>22</v>
+      </c>
+      <c r="T13" t="n">
+        <v>12109</v>
       </c>
       <c r="U13" t="inlineStr">
         <is>
@@ -1840,15 +1528,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>16009</t>
-        </is>
+      <c r="B14" t="n">
+        <v>151</v>
+      </c>
+      <c r="C14" t="n">
+        <v>16009</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1860,13 +1544,11 @@
           <t>SBST</t>
         </is>
       </c>
-      <c r="F14" s="2" t="n">
-        <v>45683.97291666667</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>16009</t>
-        </is>
+      <c r="F14" s="5" t="n">
+        <v>45684.3856712963</v>
+      </c>
+      <c r="G14" t="n">
+        <v>16009</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1875,63 +1557,43 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>SEA</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>64009</t>
-        </is>
+          <t>SDA</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" t="n">
+        <v>64009</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
           <t>SD</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>0635</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>2347</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>0634</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>2351</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>0639</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>2354</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
+      <c r="M14" t="n">
+        <v>12109</v>
+      </c>
+      <c r="N14" t="n">
+        <v>635</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2347</v>
+      </c>
+      <c r="P14" t="n">
+        <v>634</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>2351</v>
+      </c>
+      <c r="R14" t="n">
+        <v>639</v>
+      </c>
+      <c r="S14" t="n">
+        <v>2354</v>
+      </c>
+      <c r="T14" t="n">
+        <v>12109</v>
       </c>
       <c r="U14" t="inlineStr">
         <is>
@@ -1945,15 +1607,11 @@
           <t>NextBus</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>10009</t>
-        </is>
+      <c r="B15" t="n">
+        <v>75</v>
+      </c>
+      <c r="C15" t="n">
+        <v>10009</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1965,13 +1623,11 @@
           <t>SMRT</t>
         </is>
       </c>
-      <c r="F15" s="2" t="n">
-        <v>45683.96820601852</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>10009</t>
-        </is>
+      <c r="F15" s="5" t="n">
+        <v>45684.38269675926</v>
+      </c>
+      <c r="G15" t="n">
+        <v>10009</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1983,60 +1639,40 @@
           <t>SEA</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>44989</t>
-        </is>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="n">
+        <v>44989</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
           <t>SD</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>0548</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>2350</t>
-        </is>
-      </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>0546</t>
-        </is>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>2350</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>0552</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>2351</t>
-        </is>
-      </c>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>12109</t>
-        </is>
+      <c r="M15" t="n">
+        <v>12109</v>
+      </c>
+      <c r="N15" t="n">
+        <v>548</v>
+      </c>
+      <c r="O15" t="n">
+        <v>2350</v>
+      </c>
+      <c r="P15" t="n">
+        <v>546</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>2350</v>
+      </c>
+      <c r="R15" t="n">
+        <v>552</v>
+      </c>
+      <c r="S15" t="n">
+        <v>2351</v>
+      </c>
+      <c r="T15" t="n">
+        <v>12109</v>
       </c>
       <c r="U15" t="inlineStr">
         <is>
@@ -2045,7 +1681,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2055,7 +1691,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2193,7 +1829,7 @@
         </is>
       </c>
       <c r="F2" s="5" t="n">
-        <v>45683.98672453704</v>
+        <v>45684.39681712963</v>
       </c>
       <c r="G2" t="n">
         <v>53009</v>
@@ -2209,7 +1845,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
         <v>28009</v>
@@ -2272,7 +1908,7 @@
         </is>
       </c>
       <c r="F3" s="5" t="n">
-        <v>45683.9796875</v>
+        <v>45684.39141203704</v>
       </c>
       <c r="G3" t="n">
         <v>44989</v>
@@ -2295,7 +1931,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>DD</t>
         </is>
       </c>
       <c r="M3" t="n">
@@ -2351,7 +1987,7 @@
         </is>
       </c>
       <c r="F4" s="5" t="n">
-        <v>45683.99150462963</v>
+        <v>45684.3915625</v>
       </c>
       <c r="G4" t="n">
         <v>44989</v>
@@ -2367,7 +2003,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
         <v>10009</v>
@@ -2430,7 +2066,7 @@
         </is>
       </c>
       <c r="F5" s="5" t="n">
-        <v>45683.97895833333</v>
+        <v>45684.39751157408</v>
       </c>
       <c r="G5" t="n">
         <v>44989</v>
@@ -2453,7 +2089,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>DD</t>
         </is>
       </c>
       <c r="M5" t="n">
@@ -2509,7 +2145,7 @@
         </is>
       </c>
       <c r="F6" s="5" t="n">
-        <v>45683.97811342592</v>
+        <v>45684.39380787037</v>
       </c>
       <c r="G6" t="n">
         <v>11379</v>
@@ -2588,7 +2224,7 @@
         </is>
       </c>
       <c r="F7" s="5" t="n">
-        <v>45683.98077546297</v>
+        <v>45684.39166666667</v>
       </c>
       <c r="G7" t="n">
         <v>82009</v>
@@ -2604,7 +2240,7 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
         <v>43009</v>
@@ -2667,7 +2303,7 @@
         </is>
       </c>
       <c r="F8" s="5" t="n">
-        <v>45683.98350694445</v>
+        <v>45684.38679398148</v>
       </c>
       <c r="G8" t="n">
         <v>82009</v>
@@ -2746,7 +2382,7 @@
         </is>
       </c>
       <c r="F9" s="5" t="n">
-        <v>45683.98182870371</v>
+        <v>45684.39206018519</v>
       </c>
       <c r="G9" t="n">
         <v>22009</v>
@@ -2769,7 +2405,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>DD</t>
+          <t>SD</t>
         </is>
       </c>
       <c r="M9" t="n">
@@ -2825,7 +2461,7 @@
         </is>
       </c>
       <c r="F10" s="5" t="n">
-        <v>45683.97913194444</v>
+        <v>45684.39449074074</v>
       </c>
       <c r="G10" t="n">
         <v>43009</v>
@@ -2904,7 +2540,7 @@
         </is>
       </c>
       <c r="F11" s="5" t="n">
-        <v>45683.98072916667</v>
+        <v>45684.39015046296</v>
       </c>
       <c r="G11" t="n">
         <v>64009</v>
@@ -2920,14 +2556,14 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
         <v>11379</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>DD</t>
         </is>
       </c>
       <c r="M11" t="n">
@@ -2967,14 +2603,14 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>52</v>
+        <v>151</v>
       </c>
       <c r="C12" t="n">
-        <v>28009</v>
+        <v>64009</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Jurong East Int</t>
+          <t>Hougang Ctrl Int</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -2983,10 +2619,10 @@
         </is>
       </c>
       <c r="F12" s="5" t="n">
-        <v>45683.97232638889</v>
+        <v>45684.39284722223</v>
       </c>
       <c r="G12" t="n">
-        <v>28009</v>
+        <v>64009</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -3002,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>53009</v>
+        <v>16009</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
@@ -3010,32 +2646,32 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>12109</v>
+        <v>12101</v>
       </c>
       <c r="N12" t="n">
-        <v>623</v>
+        <v>642</v>
       </c>
       <c r="O12" t="n">
-        <v>23</v>
+        <v>2317</v>
       </c>
       <c r="P12" t="n">
-        <v>625</v>
+        <v>642</v>
       </c>
       <c r="Q12" t="n">
-        <v>21</v>
+        <v>2315</v>
       </c>
       <c r="R12" t="n">
-        <v>627</v>
+        <v>611</v>
       </c>
       <c r="S12" t="n">
-        <v>22</v>
+        <v>2317</v>
       </c>
       <c r="T12" t="n">
-        <v>12109</v>
+        <v>12101</v>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>Opp Ngee Ann Poly</t>
+          <t>Ngee Ann Poly</t>
         </is>
       </c>
     </row>
@@ -3046,14 +2682,14 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>151</v>
+        <v>52</v>
       </c>
       <c r="C13" t="n">
-        <v>16009</v>
+        <v>28009</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Kent Ridge Ter</t>
+          <t>Jurong East Int</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -3062,10 +2698,10 @@
         </is>
       </c>
       <c r="F13" s="5" t="n">
-        <v>45683.98357638889</v>
+        <v>45684.38995370371</v>
       </c>
       <c r="G13" t="n">
-        <v>16009</v>
+        <v>28009</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -3081,33 +2717,33 @@
         <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>64009</v>
+        <v>53009</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>DD</t>
         </is>
       </c>
       <c r="M13" t="n">
         <v>12109</v>
       </c>
       <c r="N13" t="n">
-        <v>635</v>
+        <v>623</v>
       </c>
       <c r="O13" t="n">
-        <v>2347</v>
+        <v>23</v>
       </c>
       <c r="P13" t="n">
-        <v>634</v>
+        <v>625</v>
       </c>
       <c r="Q13" t="n">
-        <v>2351</v>
+        <v>21</v>
       </c>
       <c r="R13" t="n">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="S13" t="n">
-        <v>2354</v>
+        <v>22</v>
       </c>
       <c r="T13" t="n">
         <v>12109</v>
@@ -3125,26 +2761,26 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="C14" t="n">
-        <v>10009</v>
+        <v>16009</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Bt Merah Int</t>
+          <t>Kent Ridge Ter</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>SMRT</t>
+          <t>SBST</t>
         </is>
       </c>
       <c r="F14" s="5" t="n">
-        <v>45683.9805324074</v>
+        <v>45684.38582175926</v>
       </c>
       <c r="G14" t="n">
-        <v>10009</v>
+        <v>16009</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -3160,38 +2796,117 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
+        <v>64009</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>12109</v>
+      </c>
+      <c r="N14" t="n">
+        <v>635</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2347</v>
+      </c>
+      <c r="P14" t="n">
+        <v>634</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>2351</v>
+      </c>
+      <c r="R14" t="n">
+        <v>639</v>
+      </c>
+      <c r="S14" t="n">
+        <v>2354</v>
+      </c>
+      <c r="T14" t="n">
+        <v>12109</v>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>Opp Ngee Ann Poly</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>NextBus2</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>75</v>
+      </c>
+      <c r="C15" t="n">
+        <v>10009</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Bt Merah Int</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>SMRT</t>
+        </is>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>45684.39032407408</v>
+      </c>
+      <c r="G15" t="n">
+        <v>10009</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>WAB</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>SEA</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="n">
         <v>44989</v>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>SD</t>
         </is>
       </c>
-      <c r="M14" t="n">
-        <v>12109</v>
-      </c>
-      <c r="N14" t="n">
+      <c r="M15" t="n">
+        <v>12109</v>
+      </c>
+      <c r="N15" t="n">
         <v>548</v>
       </c>
-      <c r="O14" t="n">
+      <c r="O15" t="n">
         <v>2350</v>
       </c>
-      <c r="P14" t="n">
+      <c r="P15" t="n">
         <v>546</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="Q15" t="n">
         <v>2350</v>
       </c>
-      <c r="R14" t="n">
+      <c r="R15" t="n">
         <v>552</v>
       </c>
-      <c r="S14" t="n">
+      <c r="S15" t="n">
         <v>2351</v>
       </c>
-      <c r="T14" t="n">
-        <v>12109</v>
-      </c>
-      <c r="U14" t="inlineStr">
+      <c r="T15" t="n">
+        <v>12109</v>
+      </c>
+      <c r="U15" t="inlineStr">
         <is>
           <t>Opp Ngee Ann Poly</t>
         </is>

</xml_diff>